<commit_message>
fix Joint pattern if only one side
</commit_message>
<xml_diff>
--- a/pyCGM2/Settings/jointPatterns/Nieuwenhuys2017.xlsx
+++ b/pyCGM2/Settings/jointPatterns/Nieuwenhuys2017.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLS501\Documents\Programming\API\pyCGM2\pyCGM2\pyCGM2\Settings\jointPatterns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fleboeuf\Documents\Programmation\pyCGM2\pyCGM2\pyCGM2\Settings\jointPatterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9C050C-890F-4192-AC14-EC72615AF08B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2894" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="328">
   <si>
     <t>Plan</t>
   </si>
@@ -1119,7 +1118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1709,26 +1708,26 @@
     <xf numFmtId="49" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="16" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="16" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="40 % - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="60 % - Accent1" xfId="5" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
+    <cellStyle name="Titre 3" xfId="2" builtinId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1744,7 +1743,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1819,23 +1818,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1871,23 +1853,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2063,14 +2028,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
@@ -4277,12 +4242,8 @@
       <c r="L61" s="61" t="s">
         <v>253</v>
       </c>
-      <c r="M61" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="N61" s="61" t="s">
-        <v>253</v>
-      </c>
+      <c r="M61" s="61"/>
+      <c r="N61" s="61"/>
     </row>
     <row r="62" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="49" t="s">
@@ -4319,12 +4280,8 @@
       <c r="L62" s="81" t="s">
         <v>254</v>
       </c>
-      <c r="M62" s="81" t="s">
-        <v>254</v>
-      </c>
-      <c r="N62" s="81" t="s">
-        <v>254</v>
-      </c>
+      <c r="M62" s="81"/>
+      <c r="N62" s="81"/>
     </row>
     <row r="63" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -4334,14 +4291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A80" sqref="A80:A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" style="22" customWidth="1"/>
     <col min="2" max="4" width="15" style="22" customWidth="1"/>
@@ -4379,7 +4336,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -4398,7 +4355,7 @@
       <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -4415,7 +4372,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -4432,7 +4389,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -4449,7 +4406,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B6" s="22" t="s">
@@ -4466,7 +4423,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B7" s="23" t="s">
@@ -4486,7 +4443,7 @@
       <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="22" t="s">
@@ -4507,7 +4464,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="22" t="s">
@@ -4527,7 +4484,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B10" s="100" t="s">
@@ -4549,7 +4506,7 @@
       <c r="H10" s="100"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -4573,7 +4530,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B12" s="22" t="s">
@@ -4593,7 +4550,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -4613,7 +4570,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="112" t="s">
+      <c r="A14" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B14" s="22" t="s">
@@ -4636,7 +4593,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="112" t="s">
+      <c r="A15" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="22" t="s">
@@ -4659,7 +4616,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="112" t="s">
+      <c r="A16" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B16" s="22" t="s">
@@ -4682,7 +4639,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B17" s="104" t="s">
@@ -4706,7 +4663,7 @@
       <c r="H17" s="104"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112" t="s">
+      <c r="A18" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -4728,7 +4685,7 @@
       <c r="H18" s="38"/>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="112" t="s">
+      <c r="A19" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="22" t="s">
@@ -4748,7 +4705,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="112" t="s">
+      <c r="A20" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B20" s="22" t="s">
@@ -4768,7 +4725,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -4788,7 +4745,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="112" t="s">
+      <c r="A22" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B22" s="22" t="s">
@@ -4808,7 +4765,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112" t="s">
+      <c r="A23" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="23" t="s">
@@ -4830,7 +4787,7 @@
       <c r="H23" s="100"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B24" s="22" t="s">
@@ -4852,7 +4809,7 @@
       <c r="H24" s="38"/>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="112" t="s">
+      <c r="A25" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B25" s="22" t="s">
@@ -4875,7 +4832,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="112" t="s">
+      <c r="A26" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B26" s="22" t="s">
@@ -4898,7 +4855,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="112" t="s">
+      <c r="A27" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B27" s="22" t="s">
@@ -4921,7 +4878,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="112" t="s">
+      <c r="A28" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="104" t="s">
@@ -4945,7 +4902,7 @@
       <c r="H28" s="104"/>
     </row>
     <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="112" t="s">
+      <c r="A29" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B29" s="22" t="s">
@@ -4965,7 +4922,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="112" t="s">
+      <c r="A30" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="22" t="s">
@@ -4988,7 +4945,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="112" t="s">
+      <c r="A31" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B31" s="22" t="s">
@@ -5011,7 +4968,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="112" t="s">
+      <c r="A32" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B32" s="70" t="s">
@@ -5035,7 +4992,7 @@
       <c r="H32" s="70"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="113" t="s">
+      <c r="A33" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B33" s="22" t="s">
@@ -5049,7 +5006,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="113" t="s">
+      <c r="A34" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B34" s="22" t="s">
@@ -5063,7 +5020,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="113" t="s">
+      <c r="A35" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="22" t="s">
@@ -5077,7 +5034,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="113" t="s">
+      <c r="A36" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B36" s="22" t="s">
@@ -5091,7 +5048,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="113" t="s">
+      <c r="A37" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B37" s="22" t="s">
@@ -5108,7 +5065,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="113" t="s">
+      <c r="A38" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B38" s="22" t="s">
@@ -5128,7 +5085,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="113" t="s">
+      <c r="A39" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B39" s="22" t="s">
@@ -5145,7 +5102,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="113" t="s">
+      <c r="A40" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B40" s="70" t="s">
@@ -5165,7 +5122,7 @@
       <c r="H40" s="70"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="114" t="s">
+      <c r="A41" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B41" s="22" t="s">
@@ -5181,7 +5138,7 @@
       <c r="H41" s="92"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B42" s="22" t="s">
@@ -5197,7 +5154,7 @@
       <c r="H42" s="92"/>
     </row>
     <row r="43" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="114" t="s">
+      <c r="A43" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B43" s="22" t="s">
@@ -5213,7 +5170,7 @@
       <c r="H43" s="92"/>
     </row>
     <row r="44" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="114" t="s">
+      <c r="A44" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B44" s="22" t="s">
@@ -5229,7 +5186,7 @@
       <c r="H44" s="92"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="114" t="s">
+      <c r="A45" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B45" s="22" t="s">
@@ -5248,7 +5205,7 @@
       <c r="H45" s="92"/>
     </row>
     <row r="46" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B46" s="22" t="s">
@@ -5267,7 +5224,7 @@
       <c r="H46" s="92"/>
     </row>
     <row r="47" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="114" t="s">
+      <c r="A47" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B47" s="22" t="s">
@@ -5286,7 +5243,7 @@
       <c r="H47" s="92"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="114" t="s">
+      <c r="A48" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B48" s="22" t="s">
@@ -5308,7 +5265,7 @@
       <c r="H48" s="92"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="114" t="s">
+      <c r="A49" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B49" s="22" t="s">
@@ -5331,7 +5288,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="114" t="s">
+      <c r="A50" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B50" s="70" t="s">
@@ -5355,7 +5312,7 @@
       <c r="H50" s="70"/>
     </row>
     <row r="51" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="112" t="s">
+      <c r="A51" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B51" s="22" t="s">
@@ -5376,7 +5333,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="112" t="s">
+      <c r="A52" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B52" s="22" t="s">
@@ -5396,7 +5353,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="112" t="s">
+      <c r="A53" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B53" s="22" t="s">
@@ -5416,7 +5373,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="112" t="s">
+      <c r="A54" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B54" s="22" t="s">
@@ -5440,7 +5397,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="112" t="s">
+      <c r="A55" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B55" s="22" t="s">
@@ -5460,7 +5417,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="112" t="s">
+      <c r="A56" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B56" s="22" t="s">
@@ -5480,7 +5437,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="112" t="s">
+      <c r="A57" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B57" s="22" t="s">
@@ -5503,7 +5460,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="112" t="s">
+      <c r="A58" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B58" s="22" t="s">
@@ -5526,7 +5483,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="112" t="s">
+      <c r="A59" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B59" s="22" t="s">
@@ -5549,7 +5506,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="112" t="s">
+      <c r="A60" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B60" s="104" t="s">
@@ -5573,7 +5530,7 @@
       <c r="H60" s="104"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="112" t="s">
+      <c r="A61" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B61" s="22" t="s">
@@ -5595,7 +5552,7 @@
       <c r="H61" s="38"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="112" t="s">
+      <c r="A62" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="22" t="s">
@@ -5615,7 +5572,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="112" t="s">
+      <c r="A63" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B63" s="22" t="s">
@@ -5635,7 +5592,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="112" t="s">
+      <c r="A64" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B64" s="22" t="s">
@@ -5655,7 +5612,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="112" t="s">
+      <c r="A65" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B65" s="22" t="s">
@@ -5675,7 +5632,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="112" t="s">
+      <c r="A66" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B66" s="23" t="s">
@@ -5697,7 +5654,7 @@
       <c r="H66" s="100"/>
     </row>
     <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="112" t="s">
+      <c r="A67" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B67" s="22" t="s">
@@ -5718,7 +5675,7 @@
       <c r="G67" s="38"/>
     </row>
     <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="112" t="s">
+      <c r="A68" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B68" s="22" t="s">
@@ -5741,7 +5698,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="112" t="s">
+      <c r="A69" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B69" s="22" t="s">
@@ -5764,7 +5721,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="112" t="s">
+      <c r="A70" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B70" s="22" t="s">
@@ -5787,7 +5744,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="112" t="s">
+      <c r="A71" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B71" s="104" t="s">
@@ -5811,7 +5768,7 @@
       <c r="H71" s="104"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="112" t="s">
+      <c r="A72" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B72" s="22" t="s">
@@ -5831,7 +5788,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="112" t="s">
+      <c r="A73" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B73" s="22" t="s">
@@ -5854,7 +5811,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="112" t="s">
+      <c r="A74" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B74" s="22" t="s">
@@ -5877,7 +5834,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="112" t="s">
+      <c r="A75" s="111" t="s">
         <v>84</v>
       </c>
       <c r="B75" s="70" t="s">
@@ -5901,7 +5858,7 @@
       <c r="H75" s="70"/>
     </row>
     <row r="76" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="113" t="s">
+      <c r="A76" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="22" t="s">
@@ -5918,7 +5875,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="113" t="s">
+      <c r="A77" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B77" s="22" t="s">
@@ -5938,7 +5895,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="113" t="s">
+      <c r="A78" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B78" s="22" t="s">
@@ -5955,7 +5912,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="113" t="s">
+      <c r="A79" s="112" t="s">
         <v>95</v>
       </c>
       <c r="B79" s="70" t="s">
@@ -5975,7 +5932,7 @@
       <c r="H79" s="70"/>
     </row>
     <row r="80" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="114" t="s">
+      <c r="A80" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B80" s="22" t="s">
@@ -5992,7 +5949,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="114" t="s">
+      <c r="A81" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B81" s="22" t="s">
@@ -6010,7 +5967,7 @@
       <c r="G81" s="64"/>
     </row>
     <row r="82" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="114" t="s">
+      <c r="A82" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B82" s="100" t="s">
@@ -6030,7 +5987,7 @@
       <c r="H82" s="100"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="114" t="s">
+      <c r="A83" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B83" s="22" t="s">
@@ -6051,7 +6008,7 @@
       <c r="G83" s="64"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="114" t="s">
+      <c r="A84" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B84" s="22" t="s">
@@ -6074,7 +6031,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="114" t="s">
+      <c r="A85" s="113" t="s">
         <v>230</v>
       </c>
       <c r="B85" s="70" t="s">
@@ -6113,14 +6070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C41" sqref="C41:D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -6231,10 +6188,10 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="111" t="s">
+      <c r="A12" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="111"/>
+      <c r="B12" s="114"/>
       <c r="C12" s="12" t="s">
         <v>32</v>
       </c>
@@ -6295,10 +6252,10 @@
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="111" t="s">
+      <c r="A19" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="111"/>
+      <c r="B19" s="114"/>
       <c r="C19" s="10" t="s">
         <v>18</v>
       </c>
@@ -6347,10 +6304,10 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111" t="s">
+      <c r="A25" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="111"/>
+      <c r="B25" s="114"/>
       <c r="C25" s="10" t="s">
         <v>51</v>
       </c>
@@ -6397,10 +6354,10 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="111" t="s">
+      <c r="A30" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="111"/>
+      <c r="B30" s="114"/>
       <c r="C30" s="12" t="s">
         <v>60</v>
       </c>

</xml_diff>